<commit_message>
got statistics for onehots, xls updates
</commit_message>
<xml_diff>
--- a/Training_record_onehot.xlsx
+++ b/Training_record_onehot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ronet's Corner\VIT\Capstone Project\Code\Stock Prediction using news articles on a deep learning architecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71F0A3C9-7085-4DE1-8DC2-4B0A248552E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628C64B1-EAD3-491F-AD2B-F164B834F412}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12210" yWindow="1695" windowWidth="21600" windowHeight="11385" xr2:uid="{24C04D74-E023-44AB-B1FD-AA93B56CDE60}"/>
+    <workbookView xWindow="10275" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{24C04D74-E023-44AB-B1FD-AA93B56CDE60}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>OneHot Encode</t>
   </si>
@@ -49,19 +49,27 @@
   </si>
   <si>
     <t>Train Error (cost function)</t>
+  </si>
+  <si>
+    <t>Epochs_needed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri "/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,8 +92,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,20 +411,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48F1781-99C3-4463-88DA-DEF11A7FF09F}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -429,25 +440,152 @@
       <c r="E3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>0.5</v>
+      </c>
+      <c r="B5">
+        <v>2.05E-4</v>
+      </c>
+      <c r="C5">
+        <v>5.4299999999999997E-4</v>
+      </c>
+      <c r="D5">
+        <v>122.33199999999999</v>
+      </c>
+      <c r="E5">
+        <v>6.1030000000000001E-2</v>
+      </c>
+      <c r="F5">
+        <v>13900</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>1.5</v>
+      </c>
+      <c r="B6">
+        <v>1.01E-4</v>
+      </c>
+      <c r="C6">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="D6">
+        <v>156.16540000000001</v>
+      </c>
+      <c r="E6">
+        <v>0.63890000000000002</v>
+      </c>
+      <c r="F6">
+        <v>10200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1.8599999999999999E-4</v>
-      </c>
-      <c r="C4">
-        <v>1.8599999999999999E-4</v>
-      </c>
-      <c r="D4">
-        <v>147.031722</v>
-      </c>
-      <c r="E4">
-        <v>0.60133300000000001</v>
+      <c r="B7">
+        <v>2.5900000000000001E-4</v>
+      </c>
+      <c r="C7">
+        <v>3.8210000000000002E-4</v>
+      </c>
+      <c r="D7">
+        <v>121.8057</v>
+      </c>
+      <c r="E7">
+        <v>0.61251</v>
+      </c>
+      <c r="F7">
+        <v>11600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>3.6699999999999998E-4</v>
+      </c>
+      <c r="C8">
+        <v>1.8799999999999999E-3</v>
+      </c>
+      <c r="D8">
+        <v>268.12700000000001</v>
+      </c>
+      <c r="E8">
+        <v>0.71285299999999996</v>
+      </c>
+      <c r="F8">
+        <v>33900</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="C9">
+        <v>1.5699999999999999E-4</v>
+      </c>
+      <c r="D9">
+        <v>33.376600000000003</v>
+      </c>
+      <c r="E9">
+        <v>0.66979999999999995</v>
+      </c>
+      <c r="F9">
+        <v>30800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>1.5579999999999999E-3</v>
+      </c>
+      <c r="C10">
+        <v>1.7539999999999999E-3</v>
+      </c>
+      <c r="D10">
+        <v>254.02193</v>
+      </c>
+      <c r="E10">
+        <v>0.73233099999999995</v>
+      </c>
+      <c r="F10">
+        <v>11100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>9.1600000000000004E-4</v>
+      </c>
+      <c r="C11">
+        <v>2.433E-4</v>
+      </c>
+      <c r="D11">
+        <v>39.465200000000003</v>
+      </c>
+      <c r="E11">
+        <v>0.65429999999999999</v>
+      </c>
+      <c r="F11">
+        <v>27300</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated training records, graphs needed
</commit_message>
<xml_diff>
--- a/Training_record_onehot.xlsx
+++ b/Training_record_onehot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ronet's Corner\VIT\Capstone Project\Code\Stock Prediction using news articles on a deep learning architecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628C64B1-EAD3-491F-AD2B-F164B834F412}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7716ABBB-8E2F-43D5-9EED-F5BAA4C06348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10275" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{24C04D74-E023-44AB-B1FD-AA93B56CDE60}"/>
+    <workbookView xWindow="10830" yWindow="1005" windowWidth="21600" windowHeight="11385" xr2:uid="{24C04D74-E023-44AB-B1FD-AA93B56CDE60}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>OneHot Encode</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>Epochs_needed</t>
+  </si>
+  <si>
+    <t>Label Encode</t>
+  </si>
+  <si>
+    <t>Train Error</t>
+  </si>
+  <si>
+    <t>Epoch Needed</t>
   </si>
 </sst>
 </file>
@@ -92,11 +101,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48F1781-99C3-4463-88DA-DEF11A7FF09F}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -584,6 +594,171 @@
         <v>27300</v>
       </c>
     </row>
+    <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>0.5</v>
+      </c>
+      <c r="B16">
+        <v>1.37E-4</v>
+      </c>
+      <c r="C16">
+        <v>1.0399999999999999E-4</v>
+      </c>
+      <c r="D16">
+        <v>34.959778</v>
+      </c>
+      <c r="E16">
+        <v>0.56789900000000004</v>
+      </c>
+      <c r="F16">
+        <v>7900</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>1.5</v>
+      </c>
+      <c r="B17">
+        <v>2.98E-3</v>
+      </c>
+      <c r="C17">
+        <v>1.002E-4</v>
+      </c>
+      <c r="D17">
+        <v>33.224969000000002</v>
+      </c>
+      <c r="E17">
+        <v>0.58259300000000003</v>
+      </c>
+      <c r="F17">
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>4.4200000000000001E-4</v>
+      </c>
+      <c r="C18" s="2">
+        <v>8.6299999999999997E-5</v>
+      </c>
+      <c r="D18">
+        <v>14.1225</v>
+      </c>
+      <c r="E18">
+        <v>0.58657499999999996</v>
+      </c>
+      <c r="F18">
+        <v>17900</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>7.3499999999999998E-4</v>
+      </c>
+      <c r="C19">
+        <v>1.4760000000000001E-4</v>
+      </c>
+      <c r="D19">
+        <v>54.525542999999999</v>
+      </c>
+      <c r="E19">
+        <v>0.60028700000000002</v>
+      </c>
+      <c r="F19">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>3.4699999999999998E-4</v>
+      </c>
+      <c r="C20">
+        <v>1.0730000000000001E-4</v>
+      </c>
+      <c r="D20">
+        <v>36.772277000000003</v>
+      </c>
+      <c r="E20">
+        <v>0.58668799999999999</v>
+      </c>
+      <c r="F20">
+        <v>70600</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <v>1.5510000000000001E-3</v>
+      </c>
+      <c r="C21">
+        <v>3.1970000000000002E-4</v>
+      </c>
+      <c r="D21">
+        <v>106.27934</v>
+      </c>
+      <c r="E21">
+        <v>0.63683800000000002</v>
+      </c>
+      <c r="F21">
+        <v>20700</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22">
+        <v>4.5800000000000002E-4</v>
+      </c>
+      <c r="C22">
+        <v>4.9950000000000005E-4</v>
+      </c>
+      <c r="D22">
+        <v>150.49700000000001</v>
+      </c>
+      <c r="E22">
+        <v>0.611398</v>
+      </c>
+      <c r="F22">
+        <v>65900</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>